<commit_message>
Updated metadata on spreadsheet
Added location of alignments, fastqs and pipeline scripts.
</commit_message>
<xml_diff>
--- a/Plant_Promoter_Comparison.xlsx
+++ b/Plant_Promoter_Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="1180" windowWidth="32200" windowHeight="19220" tabRatio="500"/>
+    <workbookView xWindow="2980" yWindow="580" windowWidth="32200" windowHeight="19220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Species Name</t>
   </si>
@@ -109,27 +109,53 @@
     <t>Location of Alignment File(s)</t>
   </si>
   <si>
-    <t>Location of Fastq Reads</t>
-  </si>
-  <si>
     <t>Morton et al., 2014</t>
   </si>
   <si>
     <t>Name and location of TSRchitect Pipeline</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/pipeline_scripts/Morton_At_PEAT_TSRchitect.Rscript </t>
+  </si>
+  <si>
+    <t>/scratch/rtraborn/TSRchitect_plant_results/pipeline_scripts/Mejia-Guerra_Zm_CAGE_TSRchitect.Rscript</t>
+  </si>
+  <si>
+    <t>/scratch/rtraborn/TSRchitect_plant_results/pipeline_scripts/Tokizawa_CAGE_TSRchitect.Rscript</t>
+  </si>
+  <si>
+    <t>/scratch/rtraborn/TSRchitect_plant_results/pipeline_scripts/Tokizawa_Capping_TSRchitect.Rscript</t>
+  </si>
+  <si>
+    <t>Name and location of Fastq Reads</t>
+  </si>
+  <si>
+    <t>/scratch/rtraborn/TSRchitect_plant_results/alignment_data/Tokizawa_CAGE_align.bam</t>
+  </si>
+  <si>
+    <t>/scratch/rtraborn/TSRchitect_plant_results/alignment_data/Tokizawa_Vec_Capping_align.bam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/alignment_data/Morton_At_PEAT.bam </t>
+  </si>
+  <si>
+    <t>/scratch/rtraborn/TSRchitect_plant_results/alignment_data/Zm_B73-root-1.bam, /scratch/rtraborn/TSRchitect_plant_results/alignment_data/Zm_B73-root-2.bam, /scratch/rtraborn/TSRchitect_plant_results/alignment_data/Zm_B73-shoot-1.bam,, /scratch/rtraborn/TSRchitect_plant_results/alignment_data/Zm_B73-shoot-2.bam</t>
+  </si>
+  <si>
+    <t>/scratch/rtraborn/TSRchitect_plant_results/fastq_data/Tokizawa_Vec_capping_tagdust.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/fastq_data/Tokizawa_CAGE_tagdust_READ1.fq; /scratch/rtraborn/TSRchitect_plant_results/fastq_data/Tokizawa_CAGE_tagdust_READ2.fq; </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -167,7 +193,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -448,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,9 +486,9 @@
     <col min="4" max="7" width="29.1640625" customWidth="1"/>
     <col min="8" max="8" width="29.6640625" customWidth="1"/>
     <col min="9" max="9" width="34.5" customWidth="1"/>
-    <col min="10" max="10" width="42.1640625" customWidth="1"/>
-    <col min="11" max="11" width="27.33203125" customWidth="1"/>
-    <col min="12" max="12" width="35.6640625" customWidth="1"/>
+    <col min="10" max="10" width="78.5" customWidth="1"/>
+    <col min="11" max="11" width="94.1640625" customWidth="1"/>
+    <col min="12" max="12" width="87" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -497,10 +523,10 @@
         <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -531,6 +557,15 @@
       <c r="I2" s="2">
         <v>324461</v>
       </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -560,13 +595,22 @@
       <c r="I3" s="2">
         <v>324461</v>
       </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -588,6 +632,15 @@
       </c>
       <c r="I4" s="2">
         <v>24207</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -620,6 +673,15 @@
       <c r="I5" s="2">
         <f>75681/4</f>
         <v>18920.25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Plant Promoter Comparison spreadsheet.
</commit_message>
<xml_diff>
--- a/Plant_Promoter_Comparison.xlsx
+++ b/Plant_Promoter_Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="580" windowWidth="32200" windowHeight="19220" tabRatio="500"/>
+    <workbookView xWindow="51700" yWindow="1400" windowWidth="32200" windowHeight="19220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Species Name</t>
   </si>
@@ -130,9 +130,6 @@
     <t>/scratch/rtraborn/TSRchitect_plant_results/pipeline_scripts/Tokizawa_Capping_TSRchitect.Rscript</t>
   </si>
   <si>
-    <t>Name and location of Fastq Reads</t>
-  </si>
-  <si>
     <t>/scratch/rtraborn/TSRchitect_plant_results/alignment_data/Tokizawa_CAGE_align.bam</t>
   </si>
   <si>
@@ -149,6 +146,33 @@
   </si>
   <si>
     <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/fastq_data/Tokizawa_CAGE_tagdust_READ1.fq; /scratch/rtraborn/TSRchitect_plant_results/fastq_data/Tokizawa_CAGE_tagdust_READ2.fq; </t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>cDNA</t>
+  </si>
+  <si>
+    <t>Mutliple/NA</t>
+  </si>
+  <si>
+    <t>Name and location of Original Reads</t>
+  </si>
+  <si>
+    <t>/scratch/rtraborn/TSRchitect_plant_results/Arabidopsis/EST_cDNA/ATH_EST_sequences_20101108.fas</t>
+  </si>
+  <si>
+    <t>/scratch/rtraborn/TSRchitect_plant_results/Arabidopsis/EST_cDNA/ATH_cDNA_sequences_20101108.fas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/Arabidopsis/EST_cDNA/TH_EST_sequences_20101108.gsq </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/Arabidopsis/EST_cDNA/ATH_cDNA_sequences_20101108.gsq </t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -472,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,7 +547,7 @@
         <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="L1" t="s">
         <v>20</v>
@@ -558,10 +582,10 @@
         <v>324461</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
         <v>24</v>
@@ -596,10 +620,10 @@
         <v>324461</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
         <v>25</v>
@@ -634,7 +658,7 @@
         <v>24207</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
@@ -675,13 +699,65 @@
         <v>18920.25</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" t="s">
         <v>21</v>
       </c>
       <c r="L5" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>1816638</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>78096</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data sources spreadsheet.
</commit_message>
<xml_diff>
--- a/Plant_Promoter_Comparison.xlsx
+++ b/Plant_Promoter_Comparison.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Taylor/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Taylor/Desktop/tsrchitect-figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="51700" yWindow="1400" windowWidth="32200" windowHeight="19220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Species Name</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>CAGE</t>
-  </si>
-  <si>
-    <t>Vector Capping</t>
   </si>
   <si>
     <t>Number of input reads</t>
@@ -118,36 +115,9 @@
     <t>NA</t>
   </si>
   <si>
-    <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/pipeline_scripts/Morton_At_PEAT_TSRchitect.Rscript </t>
-  </si>
-  <si>
-    <t>/scratch/rtraborn/TSRchitect_plant_results/pipeline_scripts/Mejia-Guerra_Zm_CAGE_TSRchitect.Rscript</t>
-  </si>
-  <si>
-    <t>/scratch/rtraborn/TSRchitect_plant_results/pipeline_scripts/Tokizawa_CAGE_TSRchitect.Rscript</t>
-  </si>
-  <si>
-    <t>/scratch/rtraborn/TSRchitect_plant_results/pipeline_scripts/Tokizawa_Capping_TSRchitect.Rscript</t>
-  </si>
-  <si>
-    <t>/scratch/rtraborn/TSRchitect_plant_results/alignment_data/Tokizawa_CAGE_align.bam</t>
-  </si>
-  <si>
-    <t>/scratch/rtraborn/TSRchitect_plant_results/alignment_data/Tokizawa_Vec_Capping_align.bam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/alignment_data/Morton_At_PEAT.bam </t>
-  </si>
-  <si>
-    <t>/scratch/rtraborn/TSRchitect_plant_results/alignment_data/Zm_B73-root-1.bam, /scratch/rtraborn/TSRchitect_plant_results/alignment_data/Zm_B73-root-2.bam, /scratch/rtraborn/TSRchitect_plant_results/alignment_data/Zm_B73-shoot-1.bam,, /scratch/rtraborn/TSRchitect_plant_results/alignment_data/Zm_B73-shoot-2.bam</t>
-  </si>
-  <si>
     <t>/scratch/rtraborn/TSRchitect_plant_results/fastq_data/Tokizawa_Vec_capping_tagdust.fq</t>
   </si>
   <si>
-    <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/fastq_data/Tokizawa_CAGE_tagdust_READ1.fq; /scratch/rtraborn/TSRchitect_plant_results/fastq_data/Tokizawa_CAGE_tagdust_READ2.fq; </t>
-  </si>
-  <si>
     <t>EST</t>
   </si>
   <si>
@@ -160,26 +130,120 @@
     <t>Name and location of Original Reads</t>
   </si>
   <si>
-    <t>/scratch/rtraborn/TSRchitect_plant_results/Arabidopsis/EST_cDNA/ATH_EST_sequences_20101108.fas</t>
-  </si>
-  <si>
-    <t>/scratch/rtraborn/TSRchitect_plant_results/Arabidopsis/EST_cDNA/ATH_cDNA_sequences_20101108.fas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/Arabidopsis/EST_cDNA/TH_EST_sequences_20101108.gsq </t>
-  </si>
-  <si>
-    <t xml:space="preserve">/scratch/rtraborn/TSRchitect_plant_results/Arabidopsis/EST_cDNA/ATH_cDNA_sequences_20101108.gsq </t>
-  </si>
-  <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Oligo Capping</t>
+  </si>
+  <si>
+    <t>/projects/TSRplants/ZmCAGE/alignment/Zm_B73-root-1.bam, /projects/TSRplants/ZmCAGE/alignment/Zm_B73-root-2.bam, /projects/TSRplants/ZmCAGE/alignment/Zm_B73-shoot-1.bam, //projects/TSRplants/ZmCAGE/alignment/Zm_B73-shoot-2.bam</t>
+  </si>
+  <si>
+    <t>/projects/TSRplants/AtCAGE/fastq/DRR066436_1.fastq, /projects/TSRplants/AtCAGE/fastq/DRR066436_2.fastq</t>
+  </si>
+  <si>
+    <t>/projects/TSRplants/AtCAGE/scripts/At_CAGE_TSRchitect.Rscript</t>
+  </si>
+  <si>
+    <t>/projects/TSRplants/AtPEAT/AtPEAT_TSRchitect.Rscript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/projects/TSRplants/ZmCAGE/scripts/ZmCAGE_TSRchitect.Rscript </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/projects/TSRplants/AtCAGE/alignment/AtCAGE.aligned.bam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFF4F4F4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/projects/TSRplants/AtOligo/alignment/OligoCap_align.bam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFF4F4F4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/projects/TSRplants/AtPEAT/alignment/AtPEAT.bam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFF4F4F4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>/projects/TSRplants/ESTcDNA/A_thaliana/ATH_cDNA_sequences_20101108.gsq</t>
+  </si>
+  <si>
+    <t>/projects/TSRplants/ESTcDNA/A_thaliana/reads/A_thaliana_ESTs_genbank.fasta</t>
+  </si>
+  <si>
+    <t>/projects/TSRplants/ESTcDNA/A_thaliana/reads/ATH_cDNA_sequences_20101108.fas</t>
+  </si>
+  <si>
+    <t>/projects/TSRplants/ESTcDNA/Z_mays/reads/Z_mays_ESTs_genbank.fasta</t>
+  </si>
+  <si>
+    <t>/projects/TSRplants/ESTcDNA/Z_mays/reads/cDNAzm_1.fa, /projects/TSRplants/ESTcDNA/Z_mays/reads/cDNAzm_2.fa,  /projects/TSRplants/ESTcDNA/Z_mays/reads/cDNAzm_3.fa,  /projects/TSRplants/ESTcDNA/Z_mays/reads/cDNAzm_4.fa</t>
+  </si>
+  <si>
+    <t>multiple</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -194,13 +258,31 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFF4F4F4"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,15 +294,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,10 +600,10 @@
     <col min="2" max="2" width="32.5" customWidth="1"/>
     <col min="3" max="3" width="26.83203125" customWidth="1"/>
     <col min="4" max="7" width="29.1640625" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" customWidth="1"/>
-    <col min="9" max="9" width="34.5" customWidth="1"/>
-    <col min="10" max="10" width="78.5" customWidth="1"/>
-    <col min="11" max="11" width="94.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="105.1640625" customWidth="1"/>
+    <col min="11" max="11" width="110.1640625" customWidth="1"/>
     <col min="12" max="12" width="87" customWidth="1"/>
   </cols>
   <sheetData>
@@ -526,31 +618,31 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -567,7 +659,7 @@
         <v>430630840</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -581,14 +673,14 @@
       <c r="I2" s="2">
         <v>324461</v>
       </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
+      <c r="J2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -599,13 +691,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>78194467</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -619,14 +711,14 @@
       <c r="I3" s="2">
         <v>324461</v>
       </c>
-      <c r="J3" t="s">
-        <v>27</v>
+      <c r="J3" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
         <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -634,16 +726,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>22578668</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -657,22 +749,22 @@
       <c r="I4" s="2">
         <v>24207</v>
       </c>
-      <c r="J4" t="s">
-        <v>28</v>
+      <c r="J4" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -682,7 +774,7 @@
         <v>12958666</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -699,13 +791,13 @@
         <v>18920.25</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -713,25 +805,26 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>1816638</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="4"/>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -739,25 +832,76 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>78096</v>
       </c>
       <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated information on Plant Promoter Comparison spreadsheet.
</commit_message>
<xml_diff>
--- a/Plant_Promoter_Comparison.xlsx
+++ b/Plant_Promoter_Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Species Name</t>
   </si>
@@ -231,19 +231,18 @@
   <si>
     <t>multiple</t>
   </si>
+  <si>
+    <t>/projects/TSRplants/ESTcDNA/Z_mays/alignments/cDNAzm_?.fa.gsq; /projects/TSRplants/ESTcDNA/Z_mays/alignments/cDNAzm_?.bed</t>
+  </si>
+  <si>
+    <t>/projects/TSRplants/ESTcDNA/A_thaliana/alignments/genbank_EST/AtESTgenbank_align.bed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -296,20 +295,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -590,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,6 +823,9 @@
       <c r="G6" t="s">
         <v>41</v>
       </c>
+      <c r="H6" s="7">
+        <v>16238</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" t="s">
         <v>37</v>
@@ -866,6 +870,9 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
+      <c r="D8" s="8">
+        <v>2019694</v>
+      </c>
       <c r="E8" t="s">
         <v>26</v>
       </c>
@@ -875,7 +882,9 @@
       <c r="G8" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="K8" t="s">
         <v>39</v>
       </c>
@@ -890,6 +899,9 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
+      <c r="D9" s="8">
+        <v>27455</v>
+      </c>
       <c r="E9" t="s">
         <v>26</v>
       </c>
@@ -899,7 +911,9 @@
       <c r="G9" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="K9" s="5" t="s">
         <v>40</v>
       </c>

</xml_diff>